<commit_message>
Cucumber folder structure and frame added
</commit_message>
<xml_diff>
--- a/target/test-classes/CustomerDetails.xlsx
+++ b/target/test-classes/CustomerDetails.xlsx
@@ -25,10 +25,10 @@
     <t>Phone Number</t>
   </si>
   <si>
-    <t>rupamswain1@gmail.com</t>
+    <t>cajksbcajksnckansckaskc</t>
   </si>
   <si>
-    <t>rupam123</t>
+    <t>rupamswsabsabsjxbajsx</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,18 +414,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2">
-        <v>7205320090</v>
+        <v>165445545646546</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" display="rupamswain1@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>